<commit_message>
Tess  s s s
</commit_message>
<xml_diff>
--- a/excel/ah_parties.xlsx
+++ b/excel/ah_parties.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
   <si>
     <t>الشيكل</t>
   </si>
@@ -405,6 +405,21 @@
   </si>
   <si>
     <t>مدى يورو</t>
+  </si>
+  <si>
+    <t>علاء المشهراوي</t>
+  </si>
+  <si>
+    <t>ابوانس سكيك</t>
+  </si>
+  <si>
+    <t>عبد الكريم عابدين</t>
+  </si>
+  <si>
+    <t>محمد الزين دليس</t>
+  </si>
+  <si>
+    <t>عمار ابوضاهر</t>
   </si>
 </sst>
 </file>
@@ -460,7 +475,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -472,21 +487,31 @@
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="16">
     <cellStyle name="Comma 2" xfId="2"/>
+    <cellStyle name="Comma 2 2" xfId="11"/>
     <cellStyle name="Comma 3" xfId="7"/>
+    <cellStyle name="Comma 3 2" xfId="14"/>
     <cellStyle name="Currency 2" xfId="3"/>
+    <cellStyle name="Currency 2 2" xfId="12"/>
     <cellStyle name="Currency 3" xfId="8"/>
+    <cellStyle name="Currency 3 2" xfId="15"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="4"/>
     <cellStyle name="Normal 3" xfId="1"/>
     <cellStyle name="Normal 3 2" xfId="6"/>
     <cellStyle name="عادي 2" xfId="5"/>
+    <cellStyle name="عادي 2 2" xfId="13"/>
     <cellStyle name="عادي 3" xfId="9"/>
     <cellStyle name="عادي 4" xfId="10"/>
   </cellStyles>
@@ -790,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F136"/>
+  <dimension ref="A1:F138"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F99" sqref="F99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -824,71 +849,43 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>29462</v>
-      </c>
-      <c r="D2" s="1">
-        <v>25712</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>-1550</v>
-      </c>
-      <c r="D3" s="1">
-        <v>-40</v>
-      </c>
-    </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>63</v>
+        <v>29462</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>27712</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>-45</v>
+        <v>-500</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
       </c>
       <c r="C6" s="1">
-        <v>-3275</v>
+        <v>63</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -896,27 +893,27 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
       </c>
       <c r="C7" s="1">
-        <v>0</v>
+        <v>-3345</v>
       </c>
       <c r="D7" s="1">
-        <v>0</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
       </c>
       <c r="C8" s="1">
-        <v>459</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
@@ -924,13 +921,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
       </c>
       <c r="C9" s="1">
-        <v>-33</v>
+        <v>-70000</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
@@ -938,13 +935,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
       </c>
       <c r="C10" s="1">
-        <v>804</v>
+        <v>459</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
@@ -952,13 +949,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
       </c>
       <c r="C11" s="1">
-        <v>155</v>
+        <v>-33</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
@@ -966,13 +963,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
       </c>
       <c r="C12" s="1">
-        <v>-890</v>
+        <v>1304</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
@@ -980,13 +977,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
       </c>
       <c r="C13" s="1">
-        <v>113</v>
+        <v>155</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
@@ -994,13 +991,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
       </c>
       <c r="C14" s="1">
-        <v>-300</v>
+        <v>-890</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
@@ -1008,13 +1005,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1">
-        <v>-970</v>
+        <v>0</v>
       </c>
       <c r="C15" s="1">
-        <v>0</v>
+        <v>113</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
@@ -1022,13 +1019,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16" s="1">
-        <v>-40</v>
+        <v>0</v>
       </c>
       <c r="C16" s="1">
-        <v>-115</v>
+        <v>-300</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
@@ -1036,10 +1033,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B17" s="1">
-        <v>-1320</v>
+        <v>-970</v>
       </c>
       <c r="C17" s="1">
         <v>0</v>
@@ -1050,13 +1047,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B18" s="1">
-        <v>0</v>
+        <v>-40</v>
       </c>
       <c r="C18" s="1">
-        <v>-10650</v>
+        <v>-115</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
@@ -1064,13 +1061,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B19" s="1">
-        <v>-1310</v>
+        <v>-1320</v>
       </c>
       <c r="C19" s="1">
-        <v>3792</v>
+        <v>0</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
@@ -1078,13 +1075,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1">
-        <v>-160</v>
+        <v>0</v>
       </c>
       <c r="C20" s="1">
-        <v>0</v>
+        <v>-10650</v>
       </c>
       <c r="D20" s="1">
         <v>0</v>
@@ -1092,13 +1089,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B21" s="1">
-        <v>0</v>
+        <v>-1310</v>
       </c>
       <c r="C21" s="1">
-        <v>-156</v>
+        <v>3792</v>
       </c>
       <c r="D21" s="1">
         <v>0</v>
@@ -1106,13 +1103,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B22" s="1">
-        <v>0</v>
+        <v>-160</v>
       </c>
       <c r="C22" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
@@ -1120,27 +1117,27 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
       </c>
       <c r="C23" s="1">
-        <v>4075</v>
+        <v>-156</v>
       </c>
       <c r="D23" s="1">
-        <v>-3000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B24" s="1">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="C24" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
@@ -1148,27 +1145,27 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
       </c>
       <c r="C25" s="1">
-        <v>0</v>
+        <v>4075</v>
       </c>
       <c r="D25" s="1">
-        <v>0</v>
+        <v>-3000</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B26" s="1">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="C26" s="1">
-        <v>-656</v>
+        <v>0</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
@@ -1176,13 +1173,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
       </c>
       <c r="C27" s="1">
-        <v>-1596</v>
+        <v>0</v>
       </c>
       <c r="D27" s="1">
         <v>0</v>
@@ -1190,13 +1187,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
       </c>
       <c r="C28" s="1">
-        <v>-105</v>
+        <v>-656</v>
       </c>
       <c r="D28" s="1">
         <v>0</v>
@@ -1204,13 +1201,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
       </c>
       <c r="C29" s="1">
-        <v>-6000</v>
+        <v>-1596</v>
       </c>
       <c r="D29" s="1">
         <v>0</v>
@@ -1218,13 +1215,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B30" s="1">
-        <v>-610</v>
+        <v>0</v>
       </c>
       <c r="C30" s="1">
-        <v>1868</v>
+        <v>-105</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
@@ -1232,13 +1229,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
       </c>
       <c r="C31" s="1">
-        <v>-760</v>
+        <v>-6000</v>
       </c>
       <c r="D31" s="1">
         <v>0</v>
@@ -1246,13 +1243,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B32" s="1">
-        <v>-5600</v>
+        <v>-610</v>
       </c>
       <c r="C32" s="1">
-        <v>0</v>
+        <v>1868</v>
       </c>
       <c r="D32" s="1">
         <v>0</v>
@@ -1260,13 +1257,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B33" s="1">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="C33" s="1">
-        <v>-5</v>
+        <v>-760</v>
       </c>
       <c r="D33" s="1">
         <v>0</v>
@@ -1274,13 +1271,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B34" s="1">
-        <v>-15</v>
+        <v>-5600</v>
       </c>
       <c r="C34" s="1">
-        <v>-5600</v>
+        <v>0</v>
       </c>
       <c r="D34" s="1">
         <v>0</v>
@@ -1288,13 +1285,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B35" s="1">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="C35" s="1">
-        <v>-10</v>
+        <v>-5</v>
       </c>
       <c r="D35" s="1">
         <v>0</v>
@@ -1302,13 +1299,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B36" s="1">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="C36" s="1">
-        <v>-400</v>
+        <v>-5600</v>
       </c>
       <c r="D36" s="1">
         <v>0</v>
@@ -1316,13 +1313,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B37" s="1">
         <v>0</v>
       </c>
       <c r="C37" s="1">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="D37" s="1">
         <v>0</v>
@@ -1330,13 +1327,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B38" s="1">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="C38" s="1">
-        <v>0</v>
+        <v>-400</v>
       </c>
       <c r="D38" s="1">
         <v>0</v>
@@ -1344,13 +1341,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B39" s="1">
         <v>0</v>
       </c>
       <c r="C39" s="1">
-        <v>-1500</v>
+        <v>0</v>
       </c>
       <c r="D39" s="1">
         <v>0</v>
@@ -1358,10 +1355,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B40" s="1">
-        <v>5475</v>
+        <v>-20</v>
       </c>
       <c r="C40" s="1">
         <v>0</v>
@@ -1372,13 +1369,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B41" s="1">
         <v>0</v>
       </c>
       <c r="C41" s="1">
-        <v>-9416</v>
+        <v>-1500</v>
       </c>
       <c r="D41" s="1">
         <v>0</v>
@@ -1386,10 +1383,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B42" s="1">
-        <v>-125</v>
+        <v>5475</v>
       </c>
       <c r="C42" s="1">
         <v>0</v>
@@ -1400,13 +1397,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B43" s="1">
-        <v>1200</v>
+        <v>0</v>
       </c>
       <c r="C43" s="1">
-        <v>0</v>
+        <v>-9416</v>
       </c>
       <c r="D43" s="1">
         <v>0</v>
@@ -1414,21 +1411,24 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B44" s="1">
-        <v>0</v>
+        <v>-225</v>
       </c>
       <c r="C44" s="1">
-        <v>-60</v>
+        <v>0</v>
       </c>
       <c r="D44" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="B45" s="1">
-        <v>-95</v>
+        <v>1200</v>
       </c>
       <c r="C45" s="1">
         <v>0</v>
@@ -1439,13 +1439,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B46" s="1">
         <v>0</v>
       </c>
       <c r="C46" s="1">
-        <v>-10</v>
+        <v>-60</v>
       </c>
       <c r="D46" s="1">
         <v>0</v>
@@ -1453,13 +1453,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>50</v>
+        <v>128</v>
       </c>
       <c r="B47" s="1">
-        <v>0</v>
+        <v>-95</v>
       </c>
       <c r="C47" s="1">
-        <v>-250</v>
+        <v>0</v>
       </c>
       <c r="D47" s="1">
         <v>0</v>
@@ -1467,13 +1467,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B48" s="1">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="C48" s="1">
-        <v>-2419</v>
+        <v>-10</v>
       </c>
       <c r="D48" s="1">
         <v>0</v>
@@ -1481,24 +1481,27 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B49" s="1">
-        <v>-74</v>
+        <v>0</v>
       </c>
       <c r="C49" s="1">
-        <v>0</v>
+        <v>-250</v>
       </c>
       <c r="D49" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="B50" s="1">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="C50" s="1">
-        <v>0</v>
+        <v>-2419</v>
       </c>
       <c r="D50" s="1">
         <v>0</v>
@@ -1506,13 +1509,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B51" s="1">
-        <v>0</v>
+        <v>-74</v>
       </c>
       <c r="C51" s="1">
-        <v>-300</v>
+        <v>0</v>
       </c>
       <c r="D51" s="1">
         <v>0</v>
@@ -1520,13 +1523,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="B52" s="1">
-        <v>-250</v>
+        <v>0</v>
       </c>
       <c r="C52" s="1">
-        <v>-100</v>
+        <v>-2000</v>
       </c>
       <c r="D52" s="1">
         <v>0</v>
@@ -1534,27 +1537,27 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B53" s="1">
         <v>0</v>
       </c>
       <c r="C53" s="1">
-        <v>-20925</v>
+        <v>-300</v>
       </c>
       <c r="D53" s="1">
-        <v>-20354</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B54" s="1">
-        <v>0</v>
+        <v>-250</v>
       </c>
       <c r="C54" s="1">
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="D54" s="1">
         <v>0</v>
@@ -1562,27 +1565,27 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B55" s="1">
-        <v>-14</v>
+        <v>0</v>
       </c>
       <c r="C55" s="1">
-        <v>0</v>
+        <v>-21495</v>
       </c>
       <c r="D55" s="1">
-        <v>0</v>
+        <v>-21652</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="B56" s="1">
         <v>0</v>
       </c>
       <c r="C56" s="1">
-        <v>-200</v>
+        <v>0</v>
       </c>
       <c r="D56" s="1">
         <v>0</v>
@@ -1590,13 +1593,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B57" s="1">
-        <v>0</v>
+        <v>-14</v>
       </c>
       <c r="C57" s="1">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D57" s="1">
         <v>0</v>
@@ -1604,13 +1607,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="B58" s="1">
-        <v>-600</v>
+        <v>0</v>
       </c>
       <c r="C58" s="1">
-        <v>-2522</v>
+        <v>-200</v>
       </c>
       <c r="D58" s="1">
         <v>0</v>
@@ -1618,13 +1621,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B59" s="1">
         <v>0</v>
       </c>
       <c r="C59" s="1">
-        <v>-4395</v>
+        <v>-10</v>
       </c>
       <c r="D59" s="1">
         <v>0</v>
@@ -1632,13 +1635,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B60" s="1">
-        <v>0</v>
+        <v>-600</v>
       </c>
       <c r="C60" s="1">
-        <v>-165</v>
+        <v>-2522</v>
       </c>
       <c r="D60" s="1">
         <v>0</v>
@@ -1646,13 +1649,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B61" s="1">
-        <v>6776</v>
+        <v>0</v>
       </c>
       <c r="C61" s="1">
-        <v>-967</v>
+        <v>-8965</v>
       </c>
       <c r="D61" s="1">
         <v>0</v>
@@ -1660,13 +1663,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B62" s="1">
-        <v>-389</v>
+        <v>0</v>
       </c>
       <c r="C62" s="1">
-        <v>0</v>
+        <v>-165</v>
       </c>
       <c r="D62" s="1">
         <v>0</v>
@@ -1674,27 +1677,27 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B63" s="1">
-        <v>2905</v>
+        <v>6776</v>
       </c>
       <c r="C63" s="1">
-        <v>329</v>
+        <v>-967</v>
       </c>
       <c r="D63" s="1">
-        <v>240</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B64" s="1">
-        <v>0</v>
+        <v>-389</v>
       </c>
       <c r="C64" s="1">
-        <v>-200</v>
+        <v>0</v>
       </c>
       <c r="D64" s="1">
         <v>0</v>
@@ -1702,27 +1705,27 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B65" s="1">
-        <v>0</v>
+        <v>2905</v>
       </c>
       <c r="C65" s="1">
-        <v>0</v>
+        <v>329</v>
       </c>
       <c r="D65" s="1">
-        <v>0</v>
+        <v>240</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B66" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C66" s="1">
-        <v>1124</v>
+        <v>-200</v>
       </c>
       <c r="D66" s="1">
         <v>0</v>
@@ -1730,7 +1733,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B67" s="1">
         <v>0</v>
@@ -1744,13 +1747,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B68" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C68" s="1">
-        <v>-16</v>
+        <v>1135</v>
       </c>
       <c r="D68" s="1">
         <v>0</v>
@@ -1758,7 +1761,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B69" s="1">
         <v>0</v>
@@ -1772,13 +1775,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B70" s="1">
         <v>0</v>
       </c>
       <c r="C70" s="1">
-        <v>-146</v>
+        <v>-16</v>
       </c>
       <c r="D70" s="1">
         <v>0</v>
@@ -1786,13 +1789,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B71" s="1">
         <v>0</v>
       </c>
       <c r="C71" s="1">
-        <v>-5522</v>
+        <v>0</v>
       </c>
       <c r="D71" s="1">
         <v>0</v>
@@ -1800,13 +1803,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B72" s="1">
         <v>0</v>
       </c>
       <c r="C72" s="1">
-        <v>585</v>
+        <v>-146</v>
       </c>
       <c r="D72" s="1">
         <v>0</v>
@@ -1814,24 +1817,27 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B73" s="1">
         <v>0</v>
       </c>
       <c r="C73" s="1">
-        <v>-13083</v>
+        <v>-1722</v>
       </c>
       <c r="D73" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="B74" s="1">
         <v>0</v>
       </c>
       <c r="C74" s="1">
-        <v>0</v>
+        <v>585</v>
       </c>
       <c r="D74" s="1">
         <v>0</v>
@@ -1839,13 +1845,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B75" s="1">
-        <v>-200</v>
+        <v>0</v>
       </c>
       <c r="C75" s="1">
-        <v>0</v>
+        <v>-13083</v>
       </c>
       <c r="D75" s="1">
         <v>0</v>
@@ -1853,13 +1859,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>76</v>
+        <v>130</v>
       </c>
       <c r="B76" s="1">
         <v>0</v>
       </c>
       <c r="C76" s="1">
-        <v>-6116</v>
+        <v>-330</v>
       </c>
       <c r="D76" s="1">
         <v>0</v>
@@ -1867,13 +1873,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B77" s="1">
-        <v>0</v>
+        <v>-200</v>
       </c>
       <c r="C77" s="1">
-        <v>-233</v>
+        <v>0</v>
       </c>
       <c r="D77" s="1">
         <v>0</v>
@@ -1881,13 +1887,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B78" s="1">
         <v>0</v>
       </c>
       <c r="C78" s="1">
-        <v>-40</v>
+        <v>-4750</v>
       </c>
       <c r="D78" s="1">
         <v>0</v>
@@ -1895,13 +1901,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B79" s="1">
-        <v>-150</v>
+        <v>0</v>
       </c>
       <c r="C79" s="1">
-        <v>-1074</v>
+        <v>-133</v>
       </c>
       <c r="D79" s="1">
         <v>0</v>
@@ -1909,13 +1915,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B80" s="1">
-        <v>1620</v>
+        <v>0</v>
       </c>
       <c r="C80" s="1">
-        <v>0</v>
+        <v>-40</v>
       </c>
       <c r="D80" s="1">
         <v>0</v>
@@ -1923,13 +1929,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B81" s="1">
-        <v>0</v>
+        <v>-150</v>
       </c>
       <c r="C81" s="1">
-        <v>100</v>
+        <v>-812</v>
       </c>
       <c r="D81" s="1">
         <v>0</v>
@@ -1937,13 +1943,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B82" s="1">
-        <v>0</v>
+        <v>1620</v>
       </c>
       <c r="C82" s="1">
-        <v>1070</v>
+        <v>0</v>
       </c>
       <c r="D82" s="1">
         <v>0</v>
@@ -1951,13 +1957,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B83" s="1">
         <v>0</v>
       </c>
       <c r="C83" s="1">
-        <v>-1000</v>
+        <v>100</v>
       </c>
       <c r="D83" s="1">
         <v>0</v>
@@ -1965,13 +1971,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B84" s="1">
         <v>0</v>
       </c>
       <c r="C84" s="1">
-        <v>-312</v>
+        <v>395</v>
       </c>
       <c r="D84" s="1">
         <v>0</v>
@@ -1979,13 +1985,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B85" s="1">
-        <v>-95</v>
+        <v>0</v>
       </c>
       <c r="C85" s="1">
-        <v>-200</v>
+        <v>0</v>
       </c>
       <c r="D85" s="1">
         <v>0</v>
@@ -1993,13 +1999,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B86" s="1">
         <v>0</v>
       </c>
       <c r="C86" s="1">
-        <v>8118</v>
+        <v>-312</v>
       </c>
       <c r="D86" s="1">
         <v>0</v>
@@ -2007,13 +2013,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B87" s="1">
-        <v>0</v>
+        <v>-95</v>
       </c>
       <c r="C87" s="1">
-        <v>0</v>
+        <v>-200</v>
       </c>
       <c r="D87" s="1">
         <v>0</v>
@@ -2021,13 +2027,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B88" s="1">
         <v>0</v>
       </c>
       <c r="C88" s="1">
-        <v>0</v>
+        <v>8118</v>
       </c>
       <c r="D88" s="1">
         <v>0</v>
@@ -2035,63 +2041,63 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B89" s="1">
         <v>0</v>
       </c>
       <c r="C89" s="1">
-        <v>-208</v>
+        <v>0</v>
       </c>
       <c r="D89" s="1">
-        <v>-358</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B90" s="1">
         <v>0</v>
       </c>
       <c r="C90" s="1">
-        <v>-12662</v>
+        <v>0</v>
       </c>
       <c r="D90" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="B91" s="1">
         <v>0</v>
       </c>
       <c r="C91" s="1">
-        <v>0</v>
+        <v>-208</v>
       </c>
       <c r="D91" s="1">
-        <v>0</v>
+        <v>-358</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B92" s="1">
-        <v>225</v>
+        <v>0</v>
       </c>
       <c r="C92" s="1">
-        <v>0</v>
+        <v>-12662</v>
       </c>
       <c r="D92" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="B93" s="1">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="C93" s="1">
         <v>0</v>
@@ -2102,10 +2108,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B94" s="1">
-        <v>-7</v>
+        <v>225</v>
       </c>
       <c r="C94" s="1">
         <v>0</v>
@@ -2116,13 +2122,13 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B95" s="1">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="C95" s="1">
-        <v>-21</v>
+        <v>0</v>
       </c>
       <c r="D95" s="1">
         <v>0</v>
@@ -2130,13 +2136,13 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B96" s="1">
-        <v>0</v>
+        <v>-7</v>
       </c>
       <c r="C96" s="1">
-        <v>-11563</v>
+        <v>0</v>
       </c>
       <c r="D96" s="1">
         <v>0</v>
@@ -2144,24 +2150,27 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B97" s="1">
         <v>0</v>
       </c>
       <c r="C97" s="1">
-        <v>-350</v>
+        <v>-21</v>
       </c>
       <c r="D97" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="B98" s="1">
         <v>0</v>
       </c>
       <c r="C98" s="1">
-        <v>0</v>
+        <v>-11563</v>
       </c>
       <c r="D98" s="1">
         <v>0</v>
@@ -2169,21 +2178,21 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B99" s="1">
         <v>0</v>
       </c>
       <c r="C99" s="1">
-        <v>-400</v>
+        <v>-350</v>
       </c>
       <c r="D99" s="1">
-        <v>-814</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>98</v>
+        <v>131</v>
       </c>
       <c r="B100" s="1">
         <v>0</v>
@@ -2192,32 +2201,32 @@
         <v>0</v>
       </c>
       <c r="D100" s="1">
-        <v>0</v>
+        <v>-105</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B101" s="1">
         <v>0</v>
       </c>
       <c r="C101" s="1">
-        <v>0</v>
+        <v>-400</v>
       </c>
       <c r="D101" s="1">
-        <v>0</v>
+        <v>-814</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B102" s="1">
         <v>0</v>
       </c>
       <c r="C102" s="1">
-        <v>-3102</v>
+        <v>0</v>
       </c>
       <c r="D102" s="1">
         <v>0</v>
@@ -2225,10 +2234,10 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B103" s="1">
-        <v>-50</v>
+        <v>0</v>
       </c>
       <c r="C103" s="1">
         <v>0</v>
@@ -2239,13 +2248,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B104" s="1">
         <v>0</v>
       </c>
       <c r="C104" s="1">
-        <v>-12515</v>
+        <v>-3102</v>
       </c>
       <c r="D104" s="1">
         <v>0</v>
@@ -2253,13 +2262,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B105" s="1">
-        <v>0</v>
+        <v>-50</v>
       </c>
       <c r="C105" s="1">
-        <v>-91595</v>
+        <v>0</v>
       </c>
       <c r="D105" s="1">
         <v>0</v>
@@ -2267,60 +2276,66 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B106" s="1">
+        <v>0</v>
+      </c>
+      <c r="C106" s="1">
+        <v>300</v>
+      </c>
+      <c r="D106" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B107" s="1">
+        <v>0</v>
+      </c>
+      <c r="C107" s="1">
+        <v>-32105</v>
+      </c>
+      <c r="D107" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B108" s="1">
         <v>245</v>
       </c>
-      <c r="C106" s="1">
+      <c r="C108" s="1">
         <v>-300</v>
       </c>
-      <c r="D106" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B107" s="1">
-        <v>0</v>
-      </c>
-      <c r="C107" s="1">
-        <v>0</v>
-      </c>
-      <c r="D107" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B108" s="1">
-        <v>0</v>
-      </c>
-      <c r="C108" s="1">
-        <v>0</v>
-      </c>
       <c r="D108" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="B109" s="1">
         <v>0</v>
       </c>
       <c r="C109" s="1">
-        <v>0</v>
+        <v>-508</v>
       </c>
       <c r="D109" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="B110" s="1">
         <v>0</v>
       </c>
       <c r="C110" s="1">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D110" s="1">
         <v>0</v>
@@ -2339,27 +2354,24 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B112" s="1">
-        <v>451</v>
+        <v>0</v>
       </c>
       <c r="C112" s="1">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="D112" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="B113" s="1">
         <v>0</v>
       </c>
       <c r="C113" s="1">
-        <v>-500</v>
+        <v>0</v>
       </c>
       <c r="D113" s="1">
         <v>0</v>
@@ -2367,13 +2379,13 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B114" s="1">
-        <v>0</v>
+        <v>451</v>
       </c>
       <c r="C114" s="1">
-        <v>-24520</v>
+        <v>0</v>
       </c>
       <c r="D114" s="1">
         <v>0</v>
@@ -2381,10 +2393,10 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B115" s="1">
-        <v>-1800</v>
+        <v>0</v>
       </c>
       <c r="C115" s="1">
         <v>0</v>
@@ -2395,13 +2407,13 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B116" s="1">
-        <v>2832</v>
+        <v>0</v>
       </c>
       <c r="C116" s="1">
-        <v>-277</v>
+        <v>-45349</v>
       </c>
       <c r="D116" s="1">
         <v>0</v>
@@ -2409,13 +2421,13 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B117" s="1">
-        <v>-200</v>
+        <v>-1800</v>
       </c>
       <c r="C117" s="1">
-        <v>-197</v>
+        <v>0</v>
       </c>
       <c r="D117" s="1">
         <v>0</v>
@@ -2423,13 +2435,13 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B118" s="1">
-        <v>23800</v>
+        <v>2832</v>
       </c>
       <c r="C118" s="1">
-        <v>-7682</v>
+        <v>-277</v>
       </c>
       <c r="D118" s="1">
         <v>0</v>
@@ -2437,13 +2449,13 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B119" s="1">
-        <v>0</v>
+        <v>-200</v>
       </c>
       <c r="C119" s="1">
-        <v>-57</v>
+        <v>-197</v>
       </c>
       <c r="D119" s="1">
         <v>0</v>
@@ -2451,13 +2463,13 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B120" s="1">
-        <v>-300</v>
+        <v>23800</v>
       </c>
       <c r="C120" s="1">
-        <v>0</v>
+        <v>-7682</v>
       </c>
       <c r="D120" s="1">
         <v>0</v>
@@ -2465,21 +2477,24 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B121" s="1">
         <v>0</v>
       </c>
       <c r="C121" s="1">
-        <v>-15000</v>
+        <v>-1357</v>
       </c>
       <c r="D121" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="B122" s="1">
-        <v>0</v>
+        <v>-300</v>
       </c>
       <c r="C122" s="1">
         <v>0</v>
@@ -2490,24 +2505,21 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B123" s="1">
         <v>0</v>
       </c>
       <c r="C123" s="1">
-        <v>-2930</v>
+        <v>-15000</v>
       </c>
       <c r="D123" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="B124" s="1">
-        <v>-400</v>
+        <v>0</v>
       </c>
       <c r="C124" s="1">
         <v>0</v>
@@ -2518,13 +2530,13 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B125" s="1">
-        <v>-820</v>
+        <v>0</v>
       </c>
       <c r="C125" s="1">
-        <v>0</v>
+        <v>-2880</v>
       </c>
       <c r="D125" s="1">
         <v>0</v>
@@ -2532,13 +2544,13 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B126" s="1">
-        <v>0</v>
+        <v>-400</v>
       </c>
       <c r="C126" s="1">
-        <v>678</v>
+        <v>0</v>
       </c>
       <c r="D126" s="1">
         <v>0</v>
@@ -2546,13 +2558,13 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B127" s="1">
-        <v>0</v>
+        <v>-1120</v>
       </c>
       <c r="C127" s="1">
-        <v>-168513</v>
+        <v>0</v>
       </c>
       <c r="D127" s="1">
         <v>0</v>
@@ -2560,24 +2572,27 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B128" s="1">
-        <v>-300</v>
+        <v>0</v>
       </c>
       <c r="C128" s="1">
-        <v>0</v>
+        <v>678</v>
       </c>
       <c r="D128" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>120</v>
+      </c>
       <c r="B129" s="1">
         <v>0</v>
       </c>
       <c r="C129" s="1">
-        <v>0</v>
+        <v>-149276</v>
       </c>
       <c r="D129" s="1">
         <v>0</v>
@@ -2585,13 +2600,13 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B130" s="1">
-        <v>0</v>
+        <v>-300</v>
       </c>
       <c r="C130" s="1">
-        <v>-23000</v>
+        <v>0</v>
       </c>
       <c r="D130" s="1">
         <v>0</v>
@@ -2610,27 +2625,24 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B132" s="1">
         <v>0</v>
       </c>
       <c r="C132" s="1">
-        <v>51200</v>
+        <v>-23000</v>
       </c>
       <c r="D132" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="B133" s="1">
         <v>0</v>
       </c>
       <c r="C133" s="1">
-        <v>-1478</v>
+        <v>0</v>
       </c>
       <c r="D133" s="1">
         <v>0</v>
@@ -2638,13 +2650,13 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B134" s="1">
         <v>0</v>
       </c>
       <c r="C134" s="1">
-        <v>-1220</v>
+        <v>51200</v>
       </c>
       <c r="D134" s="1">
         <v>0</v>
@@ -2652,13 +2664,13 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B135" s="1">
         <v>0</v>
       </c>
       <c r="C135" s="1">
-        <v>404900</v>
+        <v>-1478</v>
       </c>
       <c r="D135" s="1">
         <v>0</v>
@@ -2666,15 +2678,43 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B136" s="1">
+        <v>0</v>
+      </c>
+      <c r="C136" s="1">
+        <v>-1220</v>
+      </c>
+      <c r="D136" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B137" s="1">
+        <v>0</v>
+      </c>
+      <c r="C137" s="1">
+        <v>404900</v>
+      </c>
+      <c r="D137" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B136" s="1">
-        <v>0</v>
-      </c>
-      <c r="C136" s="1">
+      <c r="B138" s="1">
+        <v>0</v>
+      </c>
+      <c r="C138" s="1">
         <v>345</v>
       </c>
-      <c r="D136" s="1">
+      <c r="D138" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Test 8887 7 7
</commit_message>
<xml_diff>
--- a/excel/ah_parties.xlsx
+++ b/excel/ah_parties.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
   <si>
     <t>الشيكل</t>
   </si>
@@ -179,9 +179,6 @@
     <t>مطيع مشتهى ابورامي</t>
   </si>
   <si>
-    <t>محمد حميد</t>
-  </si>
-  <si>
     <t>باسم صافي</t>
   </si>
   <si>
@@ -254,9 +251,6 @@
     <t>ابوالحسن دغمش</t>
   </si>
   <si>
-    <t>عبد الهادي القصاص</t>
-  </si>
-  <si>
     <t>طيبه</t>
   </si>
   <si>
@@ -299,9 +293,6 @@
     <t>تيودور شحاده</t>
   </si>
   <si>
-    <t>دبي الدن</t>
-  </si>
-  <si>
     <t>الدانا</t>
   </si>
   <si>
@@ -323,9 +314,6 @@
     <t>مهند ابوخضير</t>
   </si>
   <si>
-    <t>حكيم خلف</t>
-  </si>
-  <si>
     <t>موني جرام</t>
   </si>
   <si>
@@ -335,9 +323,6 @@
     <t>ابوعلاء ابوسمهدانه</t>
   </si>
   <si>
-    <t>ريم ابوسيدو</t>
-  </si>
-  <si>
     <t>الجرجاوي ابويامن</t>
   </si>
   <si>
@@ -350,12 +335,6 @@
     <t xml:space="preserve">تامين سلطة النقد سمير حرزالله </t>
   </si>
   <si>
-    <t>باي كاش</t>
-  </si>
-  <si>
-    <t>فراس ابوكميل</t>
-  </si>
-  <si>
     <t>خالد جراده</t>
   </si>
   <si>
@@ -371,60 +350,30 @@
     <t>ابومدلله سمارت فون</t>
   </si>
   <si>
-    <t>العبادله 2</t>
-  </si>
-  <si>
     <t>علاء المشهراوي</t>
   </si>
   <si>
-    <t>ابوانس سكيك</t>
-  </si>
-  <si>
-    <t>محمد الزين دليس</t>
-  </si>
-  <si>
     <t>عمار ابوضاهر</t>
   </si>
   <si>
     <t>صندوق واحد صندوق كــــاظــــم 1 كـاظم</t>
   </si>
   <si>
-    <t>نور مشتهى</t>
-  </si>
-  <si>
-    <t>حازم مصبح</t>
-  </si>
-  <si>
     <t>صامد الشريف</t>
   </si>
   <si>
-    <t>هادي ابومعروف</t>
-  </si>
-  <si>
-    <t xml:space="preserve">حازم مشتهى </t>
-  </si>
-  <si>
     <t>سمير فتحي ساق الله</t>
   </si>
   <si>
     <t>ابواسعد حموده</t>
   </si>
   <si>
-    <t>ابوالمجد ابوعقلين</t>
-  </si>
-  <si>
     <t>احمد جوال بي</t>
   </si>
   <si>
     <t>ابودرويش</t>
   </si>
   <si>
-    <t>اكرم وادي</t>
-  </si>
-  <si>
-    <t>إبراهيم الطويل</t>
-  </si>
-  <si>
     <t>احمد خليل</t>
   </si>
   <si>
@@ -437,7 +386,40 @@
     <t>مصطفى بشير</t>
   </si>
   <si>
-    <t>محمد شيك</t>
+    <t>ام العبد الترتوري 2</t>
+  </si>
+  <si>
+    <t>عبد اللطيف عبيد</t>
+  </si>
+  <si>
+    <t>سعدو خلف</t>
+  </si>
+  <si>
+    <t>محمد شعت</t>
+  </si>
+  <si>
+    <t>ابوضياء الخالدي</t>
+  </si>
+  <si>
+    <t>فراس دير البلح</t>
+  </si>
+  <si>
+    <t>اميره الواديه</t>
+  </si>
+  <si>
+    <t>شادي ابوحصيره</t>
+  </si>
+  <si>
+    <t>حسن العبادله</t>
+  </si>
+  <si>
+    <t>الدكتور القيشاوي</t>
+  </si>
+  <si>
+    <t>محمد الخزندار</t>
+  </si>
+  <si>
+    <t>حميد</t>
   </si>
 </sst>
 </file>
@@ -833,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F138"/>
+  <dimension ref="A1:F133"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A117" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E138" sqref="E138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -869,7 +851,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -939,7 +921,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>121</v>
       </c>
       <c r="B9" s="1">
         <v>-1050</v>
@@ -1233,7 +1215,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="B30" s="1">
         <v>-300</v>
@@ -1345,7 +1327,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B38" s="1">
         <v>0</v>
@@ -1359,7 +1341,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="B39" s="1">
         <v>0</v>
@@ -1471,7 +1453,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B47" s="1">
         <v>-95</v>
@@ -1541,7 +1523,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B52" s="1">
         <v>0</v>
@@ -1597,7 +1579,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="B56" s="1">
         <v>0</v>
@@ -1611,7 +1593,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B57" s="1">
         <v>-14</v>
@@ -1625,7 +1607,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B58" s="1">
         <v>0</v>
@@ -1639,7 +1621,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B59" s="1">
         <v>0</v>
@@ -1653,7 +1635,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B60" s="1">
         <v>-625</v>
@@ -1667,7 +1649,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B61" s="1">
         <v>0</v>
@@ -1681,7 +1663,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B62" s="1">
         <v>0</v>
@@ -1695,7 +1677,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B63" s="1">
         <v>4420</v>
@@ -1709,7 +1691,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B64" s="1">
         <v>-389</v>
@@ -1723,7 +1705,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B65" s="1">
         <v>0</v>
@@ -1737,7 +1719,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B66" s="1">
         <v>0</v>
@@ -1751,7 +1733,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B67" s="1">
         <v>0</v>
@@ -1765,7 +1747,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B68" s="1">
         <v>20</v>
@@ -1779,7 +1761,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B69" s="1">
         <v>0</v>
@@ -1793,7 +1775,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B70" s="1">
         <v>0</v>
@@ -1807,7 +1789,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B71" s="1">
         <v>0</v>
@@ -1821,7 +1803,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B72" s="1">
         <v>0</v>
@@ -1835,7 +1817,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B73" s="1">
         <v>0</v>
@@ -1849,7 +1831,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B74" s="1">
         <v>1170</v>
@@ -1863,7 +1845,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B75" s="1">
         <v>0</v>
@@ -1877,7 +1859,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="B76" s="1">
         <v>0</v>
@@ -1891,7 +1873,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B77" s="1">
         <v>-200</v>
@@ -1905,7 +1887,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B78" s="1">
         <v>0</v>
@@ -1919,7 +1901,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B79" s="1">
         <v>0</v>
@@ -1933,7 +1915,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B80" s="1">
         <v>0</v>
@@ -1947,7 +1929,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="B81" s="1">
         <v>-150</v>
@@ -1961,7 +1943,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B82" s="1">
         <v>1620</v>
@@ -1975,7 +1957,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B83" s="1">
         <v>0</v>
@@ -1989,7 +1971,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B84" s="1">
         <v>0</v>
@@ -2003,7 +1985,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>77</v>
+        <v>120</v>
       </c>
       <c r="B85" s="1">
         <v>0</v>
@@ -2017,7 +1999,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B86" s="1">
         <v>0</v>
@@ -2031,7 +2013,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B87" s="1">
         <v>-95</v>
@@ -2045,7 +2027,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B88" s="1">
         <v>0</v>
@@ -2059,7 +2041,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="B89" s="1">
         <v>0</v>
@@ -2073,7 +2055,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B90" s="1">
         <v>1800</v>
@@ -2087,7 +2069,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B91" s="1">
         <v>0</v>
@@ -2101,7 +2083,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B92" s="1">
         <v>0</v>
@@ -2126,7 +2108,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B94" s="1">
         <v>200</v>
@@ -2140,7 +2122,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B95" s="1">
         <v>3000</v>
@@ -2154,7 +2136,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B96" s="1">
         <v>-7</v>
@@ -2168,7 +2150,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B97" s="1">
         <v>0</v>
@@ -2182,7 +2164,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B98" s="1">
         <v>0</v>
@@ -2196,7 +2178,7 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B99" s="1">
         <v>0</v>
@@ -2210,7 +2192,7 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B100" s="1">
         <v>0</v>
@@ -2224,7 +2206,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="B101" s="1">
         <v>0</v>
@@ -2237,9 +2219,6 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="B102" s="1">
         <v>0</v>
       </c>
@@ -2252,7 +2231,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="B103" s="1">
         <v>0</v>
@@ -2266,7 +2245,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="B104" s="1">
         <v>-222</v>
@@ -2280,7 +2259,7 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B105" s="1">
         <v>-50</v>
@@ -2294,7 +2273,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B106" s="1">
         <v>0</v>
@@ -2308,7 +2287,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B107" s="1">
         <v>0</v>
@@ -2322,7 +2301,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B108" s="1">
         <v>245</v>
@@ -2336,7 +2315,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>31</v>
+        <v>108</v>
       </c>
       <c r="B109" s="1">
         <v>0</v>
@@ -2350,7 +2329,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="B110" s="1">
         <v>0</v>
@@ -2364,7 +2343,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B111" s="1">
         <v>0</v>
@@ -2378,7 +2357,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B112" s="1">
         <v>0</v>
@@ -2392,7 +2371,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="B113" s="1">
         <v>0</v>
@@ -2406,7 +2385,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B114" s="1">
         <v>401</v>
@@ -2420,7 +2399,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B115" s="1">
         <v>0</v>
@@ -2434,7 +2413,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B116" s="1">
         <v>0</v>
@@ -2448,7 +2427,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B117" s="1">
         <v>-800</v>
@@ -2462,7 +2441,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B118" s="1">
         <v>0</v>
@@ -2476,7 +2455,7 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="B119" s="1">
         <v>0</v>
@@ -2490,7 +2469,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B120" s="1">
         <v>23800</v>
@@ -2504,7 +2483,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B121" s="1">
         <v>-1845</v>
@@ -2518,7 +2497,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B122" s="1">
         <v>-300</v>
@@ -2532,7 +2511,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B123" s="1">
         <v>0</v>
@@ -2546,7 +2525,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B124" s="1">
         <v>0</v>
@@ -2560,7 +2539,7 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="B125" s="1">
         <v>0</v>
@@ -2574,7 +2553,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="B126" s="1">
         <v>0</v>
@@ -2588,7 +2567,7 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B127" s="1">
         <v>-800</v>
@@ -2602,7 +2581,7 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="B128" s="1">
         <v>0</v>
@@ -2616,7 +2595,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B129" s="1">
         <v>0</v>
@@ -2630,7 +2609,7 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B130" s="1">
         <v>0</v>
@@ -2644,7 +2623,7 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B131" s="1">
         <v>0</v>
@@ -2658,7 +2637,7 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="B132" s="1">
         <v>0</v>
@@ -2672,7 +2651,7 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B133" s="1">
         <v>0</v>
@@ -2682,37 +2661,6 @@
       </c>
       <c r="D133" s="1">
         <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C134" s="1">
-        <v>0</v>
-      </c>
-      <c r="D134" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>